<commit_message>
atualização do dia 31/10
</commit_message>
<xml_diff>
--- a/schedule/gantt-chart.xlsx
+++ b/schedule/gantt-chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Arquivos\Documentos\unicamp\feec\ea872\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D92C75-1C78-4356-833F-2374CB882CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC579490-B00D-499D-8489-5FBE53A2B712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,6 +771,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -792,41 +804,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1285,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="33" t="s">
@@ -1492,12 +1492,14 @@
       <c r="C5" s="17">
         <v>2</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
       <c r="E5" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1510,12 +1512,14 @@
       <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
       <c r="E6" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:40" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1559,17 +1563,19 @@
         <v>19</v>
       </c>
       <c r="B9" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="17">
         <v>3</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
       <c r="E9" s="17">
         <v>0</v>
       </c>
       <c r="F9" s="18">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:40" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1743,7 @@
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:V12"/>
+      <selection activeCell="B6" sqref="B6:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1748,134 +1754,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="51" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
     </row>
     <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
     </row>
     <row r="5" spans="1:25" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
       <c r="Q5" s="45"/>
       <c r="R5" s="46"/>
       <c r="S5" s="46"/>
@@ -1887,23 +1893,23 @@
       <c r="A6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
       <c r="Q6" s="45"/>
       <c r="R6" s="46"/>
       <c r="S6" s="46"/>
@@ -1915,23 +1921,23 @@
       <c r="A7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="63"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
       <c r="Q7" s="45"/>
       <c r="R7" s="46"/>
       <c r="S7" s="46"/>
@@ -1943,23 +1949,23 @@
       <c r="A8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="46"/>
       <c r="S8" s="46"/>
@@ -1971,23 +1977,23 @@
       <c r="A9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
       <c r="Q9" s="45"/>
       <c r="R9" s="46"/>
       <c r="S9" s="46"/>
@@ -1999,23 +2005,23 @@
       <c r="A10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="46"/>
       <c r="S10" s="46"/>
@@ -2028,23 +2034,23 @@
       <c r="A11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
       <c r="Q11" s="45"/>
       <c r="R11" s="46"/>
       <c r="S11" s="46"/>

</xml_diff>